<commit_message>
update pre sit onefly
</commit_message>
<xml_diff>
--- a/Traveloka_DataAutomation_Portal_Onefly/Data/Config.xlsx
+++ b/Traveloka_DataAutomation_Portal_Onefly/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kalyana\dataautomation_personal\Traveloka_DataAutomation_Portal_Kpay\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A8AD2CA-0CFB-473B-A30D-D495FAA19B22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C45406D-E36F-48DC-93A8-A7D4C3DBAC45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3960" yWindow="1932" windowWidth="21588" windowHeight="10644" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3960" yWindow="1932" windowWidth="21588" windowHeight="10644" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -185,6 +185,9 @@
     <t>PathSAKey</t>
   </si>
   <si>
+    <t>[Dev] RPA_Moon_UploadBucket</t>
+  </si>
+  <si>
     <t>OrchestratorQueueName</t>
   </si>
   <si>
@@ -194,6 +197,21 @@
     <t>DialogDownloadChrome</t>
   </si>
   <si>
+    <t>[Dev] RPA_Moon_PathMasterFolder</t>
+  </si>
+  <si>
+    <t>[Dev] RPA_Moon_PathMailTemplate</t>
+  </si>
+  <si>
+    <t>[Dev] RPA_Moon_PathSaKey</t>
+  </si>
+  <si>
+    <t>[Dev] RPA_Moon_PathDownloadChrome</t>
+  </si>
+  <si>
+    <t>[Dev] RPA_Moon_DialogDownloadChrome</t>
+  </si>
+  <si>
     <t>SenderName</t>
   </si>
   <si>
@@ -203,25 +221,7 @@
     <t>RPA_Moon_Cred_Gmail</t>
   </si>
   <si>
-    <t>RPA_Moon_SheetIdConfig_Transport</t>
-  </si>
-  <si>
-    <t>RPA_Moon_PathMasterFolder</t>
-  </si>
-  <si>
-    <t>RPA_Moon_PathMailTemplate</t>
-  </si>
-  <si>
-    <t>RPA_Moon_PathSaKey</t>
-  </si>
-  <si>
-    <t>RPA_Moon_PathDownloadChrome</t>
-  </si>
-  <si>
-    <t>RPA_Moon_DialogDownloadChrome</t>
-  </si>
-  <si>
-    <t>RPA_Moon_UploadBucket</t>
+    <t>[Dev] RPA_Moon_SheetIdConfig_Transport</t>
   </si>
 </sst>
 </file>
@@ -648,10 +648,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>62</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -689,7 +689,7 @@
         <v>44</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C7" t="s">
         <v>45</v>
@@ -1694,7 +1694,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -2857,8 +2857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -2910,7 +2910,7 @@
         <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
@@ -2918,7 +2918,7 @@
         <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
@@ -2926,7 +2926,7 @@
         <v>46</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
@@ -2934,31 +2934,31 @@
         <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B8" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>